<commit_message>
feat: accomplish the controller of shift and schedule
</commit_message>
<xml_diff>
--- a/src/test/resources/客流数据.xlsx
+++ b/src/test/resources/客流数据.xlsx
@@ -1300,7 +1300,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1338,7 +1338,7 @@
         <v>45292.333333333336</v>
       </c>
       <c r="D2" s="5">
-        <v>45292.458333333336</v>
+        <v>45292.5</v>
       </c>
       <c r="E2" s="6">
         <v>13.4</v>
@@ -1352,10 +1352,10 @@
         <v>45056</v>
       </c>
       <c r="C3" s="9">
-        <v>45292.458333333336</v>
+        <v>45292.5</v>
       </c>
       <c r="D3" s="9">
-        <v>45292.583333333336</v>
+        <v>45292.625</v>
       </c>
       <c r="E3" s="10">
         <v>26.9</v>
@@ -1369,10 +1369,10 @@
         <v>45056</v>
       </c>
       <c r="C4" s="9">
-        <v>45292.583333333336</v>
+        <v>45292.625</v>
       </c>
       <c r="D4" s="9">
-        <v>45292.708333333336</v>
+        <v>45292.75</v>
       </c>
       <c r="E4" s="10">
         <v>18.3</v>
@@ -1386,31 +1386,21 @@
         <v>45056</v>
       </c>
       <c r="C5" s="9">
-        <v>45292.708333333336</v>
+        <v>45292.75</v>
       </c>
       <c r="D5" s="9">
-        <v>45292.833333333336</v>
+        <v>45292.875</v>
       </c>
       <c r="E5" s="10">
         <v>8.300000000000001</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="7">
-        <v>1</v>
-      </c>
-      <c r="B6" s="8">
-        <v>45056</v>
-      </c>
-      <c r="C6" s="9">
-        <v>45292.833333333336</v>
-      </c>
-      <c r="D6" s="9">
-        <v>45292.875</v>
-      </c>
-      <c r="E6" s="10">
-        <v>0.1</v>
-      </c>
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" s="11"/>
@@ -1516,13 +1506,6 @@
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>

<commit_message>
fix: fix some bug
</commit_message>
<xml_diff>
--- a/src/test/resources/客流数据.xlsx
+++ b/src/test/resources/客流数据.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>门店 ID</t>
   </si>
@@ -26,6 +26,18 @@
   </si>
   <si>
     <t>预测顾客流量</t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>15:00</t>
+  </si>
+  <si>
+    <t>18:00</t>
   </si>
 </sst>
 </file>
@@ -204,7 +216,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -220,6 +232,9 @@
     <xf numFmtId="59" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="20" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -230,6 +245,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="59" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1334,178 +1352,178 @@
       <c r="B2" s="4">
         <v>45056</v>
       </c>
-      <c r="C2" s="5">
-        <v>45292.333333333336</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="C2" t="s" s="5">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6">
         <v>45292.5</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="7">
         <v>13.4</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="7">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="9">
         <v>45056</v>
       </c>
-      <c r="C3" s="9">
-        <v>45292.5</v>
-      </c>
-      <c r="D3" s="9">
+      <c r="C3" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="D3" s="11">
         <v>45292.625</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="12">
         <v>26.9</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="7">
+      <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="9">
         <v>45056</v>
       </c>
-      <c r="C4" s="9">
-        <v>45292.625</v>
-      </c>
-      <c r="D4" s="9">
+      <c r="C4" t="s" s="10">
+        <v>7</v>
+      </c>
+      <c r="D4" s="11">
         <v>45292.75</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="12">
         <v>18.3</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="7">
+      <c r="A5" s="8">
         <v>1</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="9">
         <v>45056</v>
       </c>
-      <c r="C5" s="9">
-        <v>45292.75</v>
-      </c>
-      <c r="D5" s="9">
+      <c r="C5" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="D5" s="11">
         <v>45292.875</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="12">
         <v>8.300000000000001</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>